<commit_message>
Added Full BOM and gerber
</commit_message>
<xml_diff>
--- a/gerber/Interface_PCB_BOM.xlsx
+++ b/gerber/Interface_PCB_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\parikshit\Interface Board\Final Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\parikshit\Interface Board\Final Design\gerber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B412C38-1E91-4DFC-ABF0-9C2E65A65D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D4166-1C21-4BC0-8D9B-871E250FC392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Supplier and ref</t>
   </si>
   <si>
-    <t>I2C2,USART2,I2C1,USART1</t>
-  </si>
-  <si>
     <t>502382-0470</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>1u</t>
   </si>
   <si>
-    <t>SPI</t>
-  </si>
-  <si>
     <t>Micro_SD_Card</t>
   </si>
   <si>
@@ -187,18 +181,12 @@
     <t>AMS1117-3.3</t>
   </si>
   <si>
-    <t>JTAG</t>
-  </si>
-  <si>
     <t>FTSH10501LDVK</t>
   </si>
   <si>
     <t>AVR-JTAG-10</t>
   </si>
   <si>
-    <t>USB</t>
-  </si>
-  <si>
     <t>GMCB05B11124H1EU</t>
   </si>
   <si>
@@ -295,9 +283,6 @@
     <t>mouser - https://www.mouser.in/ProductDetail/Littelfuse/AQ1205-01ETG?qs=TCDPyi3sCW2VfoQH%2FYUj8g%3D%3D</t>
   </si>
   <si>
-    <t>VEXT</t>
-  </si>
-  <si>
     <t>PinHeader</t>
   </si>
   <si>
@@ -305,6 +290,21 @@
   </si>
   <si>
     <t>mouser - https://www.mouser.in/ProductDetail/Harwin/M20-9990246?qs=Jph8NoUxIfWjw4WmyRvzag%3D%3D</t>
+  </si>
+  <si>
+    <t>J1,J2,J3,J4</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,16 +714,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -734,16 +734,16 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,13 +754,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -771,16 +771,16 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -791,16 +791,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,16 +811,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -831,16 +831,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -851,16 +851,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1">
         <v>693072010801</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,16 +871,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,16 +891,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -911,16 +911,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -931,16 +931,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -951,16 +951,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,16 +971,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -991,16 +991,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1011,16 +1011,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1031,16 +1031,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1051,16 +1051,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1071,16 +1071,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1091,16 +1091,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1111,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1131,16 +1131,16 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1151,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1168,16 +1168,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1188,16 +1188,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated inductor and USB according to manufacturer
</commit_message>
<xml_diff>
--- a/gerber/Interface_PCB_BOM.xlsx
+++ b/gerber/Interface_PCB_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\parikshit\Interface Board\Final Design\gerber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D4166-1C21-4BC0-8D9B-871E250FC392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F6D671-66B9-409F-B783-2EFED25F97F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -268,9 +268,6 @@
     <t>LR1,LMS1</t>
   </si>
   <si>
-    <t>mouser - https://www.mouser.in/ProductDetail/Coilcraft/0805CS-390XGLC?qs=JVZp5BaCFzhiwXQ6Bmpvlg%3D%3D</t>
-  </si>
-  <si>
     <t>DEXT1</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>J8</t>
+  </si>
+  <si>
+    <t>mouser - https://www.mouser.in/ProductDetail/ABRACON/AIMC-0805-39NJ-T?qs=1vO2EIVe%252BY6yKg%252Bn%252BCAmog%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,7 +714,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1">
         <v>693072010801</v>
@@ -1060,7 +1060,7 @@
         <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
         <v>53</v>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
         <v>55</v>
@@ -1168,16 +1168,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1188,16 +1188,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
         <v>87</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>